<commit_message>
Describe the monitoring item "Execution result of gfmdhost -1 command on each gfmd" and the trigger "Multiple master gfmds ({ITEM.LASTVALUE})". (added by #778)
git-svn-id: https://svn.code.sf.net/p/gfarm/code/gfarm_zabbix/trunk@9555 4a5e1ece-6a47-475c-b646-731d720b41d0
</commit_message>
<xml_diff>
--- a/doc/ja/gfarm_monitoring_item_list.xlsx
+++ b/doc/ja/gfarm_monitoring_item_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr checkCompatibility="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-kasahr\Documents\gfarm-zabbix\doc\ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-kasahr\Documents\gfarm-zabbix\gfarm_zabbix\doc\ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="8472" windowHeight="4728" tabRatio="611" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="36" windowWidth="8472" windowHeight="4728" tabRatio="611"/>
   </bookViews>
   <sheets>
     <sheet name="テンプレート一覧" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="175">
   <si>
     <t>警告</t>
     <rPh sb="0" eb="2">
@@ -217,21 +217,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>合計</t>
-  </si>
-  <si>
-    <t>平均</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>累計</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>データの個数</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Template_Gfarm_gfmd_nodep</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1051,10 +1036,6 @@
   </si>
   <si>
     <t>{$NODATA_TIMEOUT}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{$GFSD_HOSTNAME}</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1375,6 +1356,47 @@
 (5分)</t>
     <rPh sb="5" eb="6">
       <t>プン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{$GFSD_HOSTNAMES}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Execution result of gfmdhost -1 command on each gfmd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Multiple master gfmds ({ITEM.LASTVALUE})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Multiple master gfmds ({ITEM.LASTVALUE})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"gfmdhost -1" コマンドを各gfmd上で実行したが、自分がmasterだと思っているgfmdが2台以上いた。</t>
+    <rPh sb="19" eb="20">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ジブン</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>オモ</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>イジョウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1927,11 +1949,11 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C10" sqref="C10"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="A3:B3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1942,7 +1964,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -1958,7 +1980,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
@@ -1966,15 +1988,15 @@
         <v>24</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
@@ -1982,15 +2004,15 @@
         <v>28</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
@@ -1998,57 +2020,57 @@
         <v>29</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2065,13 +2087,13 @@
     <outlinePr applyStyles="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D7" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C10" sqref="C10"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2084,7 +2106,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -2092,13 +2114,13 @@
         <v>22</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -2106,13 +2128,13 @@
         <v>23</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="24" x14ac:dyDescent="0.15">
@@ -2120,13 +2142,13 @@
         <v>23</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="24" x14ac:dyDescent="0.15">
@@ -2134,13 +2156,13 @@
         <v>23</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="24" x14ac:dyDescent="0.15">
@@ -2148,13 +2170,13 @@
         <v>23</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="36" x14ac:dyDescent="0.15">
@@ -2162,13 +2184,13 @@
         <v>23</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="36" x14ac:dyDescent="0.15">
@@ -2176,13 +2198,13 @@
         <v>23</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="24" x14ac:dyDescent="0.15">
@@ -2190,13 +2212,13 @@
         <v>23</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="24" x14ac:dyDescent="0.15">
@@ -2204,13 +2226,13 @@
         <v>23</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
@@ -2218,13 +2240,13 @@
         <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="24" x14ac:dyDescent="0.15">
@@ -2232,13 +2254,13 @@
         <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
@@ -2246,13 +2268,13 @@
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.15">
@@ -2260,13 +2282,13 @@
         <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="36" x14ac:dyDescent="0.15">
@@ -2274,69 +2296,69 @@
         <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="24" x14ac:dyDescent="0.15">
       <c r="A18" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.15">
       <c r="A20" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2353,13 +2375,13 @@
     <outlinePr applyStyles="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C10" sqref="C10"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2395,10 +2417,10 @@
         <v>27</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -2416,7 +2438,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G4" s="13"/>
     </row>
@@ -2435,7 +2457,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G5" s="13"/>
     </row>
@@ -2456,7 +2478,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G6" s="13"/>
     </row>
@@ -2475,7 +2497,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G7" s="8"/>
     </row>
@@ -2494,7 +2516,7 @@
         <v>21</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G8" s="8"/>
     </row>
@@ -2503,7 +2525,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>18</v>
@@ -2515,7 +2537,7 @@
         <v>21</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G9" s="8"/>
     </row>
@@ -2536,7 +2558,7 @@
         <v>21</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G10" s="8"/>
     </row>
@@ -2555,7 +2577,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G11" s="8"/>
     </row>
@@ -2574,7 +2596,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G12" s="8"/>
     </row>
@@ -2593,7 +2615,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G13" s="8"/>
     </row>
@@ -2610,7 +2632,7 @@
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G14" s="14"/>
     </row>
@@ -2626,10 +2648,10 @@
         <v>300</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G15" s="17"/>
     </row>
@@ -2645,10 +2667,10 @@
         <v>300</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G16" s="17"/>
     </row>
@@ -2664,107 +2686,107 @@
         <v>300</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="14"/>
+        <v>54</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="20" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14">
         <v>300</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>62</v>
+        <v>172</v>
       </c>
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="3">
+      <c r="A19" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14">
         <v>300</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="17"/>
+      <c r="E19" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="17"/>
+        <v>30</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D20" s="3">
-        <v>3600</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>46</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E20" s="17"/>
       <c r="F20" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>100</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G20" s="17"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="3">
-        <v>300</v>
+        <v>3600</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="17"/>
+        <v>52</v>
+      </c>
+      <c r="G21" s="25"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C22" s="17"/>
       <c r="D22" s="3">
-        <v>3600</v>
-      </c>
-      <c r="E22" s="17"/>
+        <v>300</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>43</v>
+      </c>
       <c r="F22" s="17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G22" s="17"/>
     </row>
@@ -2773,131 +2795,150 @@
         <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>33</v>
+        <v>14</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="D23" s="3">
-        <v>600</v>
+        <v>3600</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G23" s="17"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="14">
-        <v>300</v>
-      </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" s="14"/>
+      <c r="A24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="3">
+        <v>600</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="17"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="14"/>
+        <v>30</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="D25" s="14">
-        <v>3600</v>
-      </c>
-      <c r="E25" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>41</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C26" s="14"/>
       <c r="D26" s="14">
         <v>3600</v>
       </c>
-      <c r="E26" s="14"/>
+      <c r="E26" s="24" t="s">
+        <v>44</v>
+      </c>
       <c r="F26" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="D27" s="14">
-        <v>300</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>50</v>
-      </c>
+        <v>3600</v>
+      </c>
+      <c r="E27" s="14"/>
       <c r="F27" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B28" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14">
+        <v>300</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="14">
+      <c r="C29" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="14">
         <v>600</v>
       </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="3">
+      <c r="E29" s="14"/>
+      <c r="F29" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="14"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="3">
         <v>300</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G29" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2913,13 +2954,13 @@
     <outlinePr applyStyles="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C10" sqref="C10"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2934,7 +2975,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C1" s="12"/>
     </row>
@@ -2946,16 +2987,16 @@
         <v>4</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.15">
@@ -2963,13 +3004,13 @@
         <v>23</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="14"/>
@@ -2979,13 +3020,13 @@
         <v>23</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="14"/>
@@ -2995,13 +3036,13 @@
         <v>23</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="14"/>
@@ -3011,13 +3052,13 @@
         <v>23</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="14"/>
@@ -3027,13 +3068,13 @@
         <v>23</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="14"/>
@@ -3043,13 +3084,13 @@
         <v>23</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="14"/>
@@ -3059,13 +3100,13 @@
         <v>23</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="14"/>
@@ -3075,13 +3116,13 @@
         <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="17"/>
@@ -3091,36 +3132,36 @@
         <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A13" s="20" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>62</v>
+        <v>173</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>120</v>
+        <v>174</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
         <v>28</v>
       </c>
@@ -3131,43 +3172,43 @@
         <v>2</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="36" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-    </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+        <v>116</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+      <c r="A15" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="36" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>116</v>
+      <c r="D16" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
@@ -3177,144 +3218,160 @@
         <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>1</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="22" t="s">
-        <v>107</v>
+      <c r="D18" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="36" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>2</v>
+        <v>76</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A20" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="A20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>1</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="36" x14ac:dyDescent="0.15">
       <c r="A24" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>2</v>
+        <v>51</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>77</v>
+      <c r="A25" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
+      <c r="D25" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
implement #999 - differentiate PostgreSQL access timeout from server stop
git-svn-id: https://svn.code.sf.net/p/gfarm/code/gfarm_zabbix/trunk@10551 4a5e1ece-6a47-475c-b646-731d720b41d0
</commit_message>
<xml_diff>
--- a/doc/ja/gfarm_monitoring_item_list.xlsx
+++ b/doc/ja/gfarm_monitoring_item_list.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="198">
   <si>
     <t>警告</t>
     <rPh sb="0" eb="2">
@@ -85,10 +85,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>CPU(s) load</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Cached memory size</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -97,10 +93,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Host local time</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Memory size of kernel buffers</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -114,10 +106,6 @@
   </si>
   <si>
     <t>Free disk space on $1 in %</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Internal error message in log file $1</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -128,10 +116,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>$1 = {$MONITOR_DIR}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>$1 = {$KERNEL_LOGFILE}</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -153,15 +137,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>テンプレート</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Template_Gfarm_common_nodep</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -512,13 +488,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>psql コマンドを実行したが、正常終了しなかった。</t>
-    <rPh sb="16" eb="20">
-      <t>セイジョウシュウリョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ログファイル {$KERNEL_LOGFILE} に、正規表現 "kernel:\s.*I/O\serror" にマッチする行が見つかった。</t>
     <rPh sb="27" eb="31">
       <t>セイキヒョウゲン</t>
@@ -1514,6 +1483,36 @@
     </rPh>
     <rPh sb="78" eb="79">
       <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PostgreSQL server running</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gfarm_gfmd_postgresql_alive.sh</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PostgreSQL server access is timed out</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PostgreSQL server access is timed out</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>psql コマンドを実行したが、正常終了しなかったかタイムアウトした。</t>
+    <rPh sb="16" eb="20">
+      <t>セイジョウシュウリョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PostgreSQL デーモン・プロセスが存在しない</t>
+    <rPh sb="21" eb="23">
+      <t>ソンザイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1557,7 +1556,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1573,12 +1572,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1641,7 +1634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1675,14 +1668,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1697,10 +1689,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2078,84 +2070,84 @@
   <sheetData>
     <row r="1" spans="1:2" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="23" t="s">
+      <c r="A3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>75</v>
+      <c r="A5" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>73</v>
+      <c r="A7" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>154</v>
+      <c r="A9" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>155</v>
+      <c r="A11" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2191,245 +2183,245 @@
   <sheetData>
     <row r="1" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="23" t="s">
+      <c r="A3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>97</v>
+      <c r="D3" s="22" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="36" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>161</v>
+        <v>151</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="36" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>162</v>
+        <v>153</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>106</v>
+      <c r="A6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="36" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>131</v>
+        <v>123</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>106</v>
+      <c r="A9" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="24" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>109</v>
+      <c r="A10" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="36" x14ac:dyDescent="0.15">
-      <c r="A11" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>135</v>
+      <c r="A11" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>110</v>
+        <v>122</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="24" x14ac:dyDescent="0.15">
+      <c r="A14" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="24" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>110</v>
+      <c r="D14" s="28" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>112</v>
+      <c r="A15" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="24" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>108</v>
+        <v>119</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="24" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>110</v>
+        <v>125</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="24" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="24" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="29" t="s">
         <v>104</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2446,10 +2438,10 @@
     <outlinePr applyStyles="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C10" sqref="C10"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight"/>
@@ -2468,745 +2460,606 @@
   <sheetData>
     <row r="1" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.15">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
+        <v>300</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>300</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <v>3600</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3">
+        <v>600</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3">
+        <v>600</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13">
+        <v>3600</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13">
         <v>300</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E10" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8">
-        <v>300</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="8">
-        <v>3600</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8">
-        <v>300</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8">
-        <v>300</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="8">
+      <c r="C11" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="13">
         <v>600</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="8">
-        <v>600</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8">
-        <v>300</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="8"/>
+      <c r="F11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3">
-        <v>300</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="A12" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="13">
+        <v>600</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>141</v>
+        <v>64</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3">
-        <v>3600</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>38</v>
+        <v>300</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>28</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="3">
-        <v>600</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>181</v>
+        <v>300</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="3">
+        <v>300</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13">
+        <v>3600</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13">
+        <v>3600</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="13">
         <v>600</v>
       </c>
-      <c r="E15" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14">
-        <v>3600</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14">
-        <v>300</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="14">
+      <c r="E18" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="13">
         <v>600</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="14">
-        <v>600</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="14"/>
+      <c r="E19" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3">
-        <v>300</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="33" t="s">
-        <v>78</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="13">
+        <v>600</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>165</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3">
         <v>300</v>
       </c>
-      <c r="E21" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>52</v>
+      <c r="E21" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>168</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3">
         <v>300</v>
       </c>
-      <c r="E22" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>138</v>
+      <c r="E22" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>50</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14">
-        <v>3600</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="14"/>
+      <c r="A23" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3">
+        <v>300</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14">
-        <v>3600</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="14"/>
+      <c r="A24" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3">
+        <v>300</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="14">
-        <v>600</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F25" s="34" t="s">
-        <v>61</v>
+        <v>7</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
+        <v>300</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>50</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="14">
-        <v>600</v>
-      </c>
-      <c r="E26" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F26" s="34" t="s">
-        <v>173</v>
+        <v>10</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3">
+        <v>300</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>50</v>
       </c>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="14">
-        <v>600</v>
-      </c>
-      <c r="E27" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F27" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="G27" s="3"/>
+      <c r="A27" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="13">
+        <v>3600</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="C28" s="3"/>
       <c r="D28" s="3">
+        <v>3600</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" s="8">
         <v>300</v>
       </c>
-      <c r="E28" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F28" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="E29" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3">
+      <c r="C30" s="7"/>
+      <c r="D30" s="8">
         <v>300</v>
       </c>
-      <c r="E29" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F29" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3">
+      <c r="E30" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8">
         <v>300</v>
       </c>
-      <c r="E30" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F30" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A31" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3">
-        <v>300</v>
-      </c>
-      <c r="E31" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F31" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G31" s="3"/>
+      <c r="E31" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A32" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3">
-        <v>300</v>
-      </c>
-      <c r="E32" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F32" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3">
-        <v>300</v>
-      </c>
-      <c r="E33" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F33" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A34" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" s="14">
+      <c r="A32" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="8">
         <v>3600</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E32" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A35" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="D35" s="3">
-        <v>3600</v>
-      </c>
-      <c r="E35" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G35" s="15"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A36" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D36" s="8">
-        <v>300</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A37" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8">
-        <v>300</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A38" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="8">
-        <v>300</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A39" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D39" s="8">
-        <v>3600</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G39" s="8"/>
+      <c r="F32" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G32" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -3222,10 +3075,10 @@
     <outlinePr applyStyles="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C10" sqref="C10"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight"/>
@@ -3243,467 +3096,483 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C1" s="12"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.15">
-      <c r="A3" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>68</v>
+      <c r="C3" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>182</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>2</v>
+        <v>195</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="36" x14ac:dyDescent="0.15">
-      <c r="A9" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="16" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+      <c r="A10" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="16" t="s">
+      <c r="D10" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A11" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A11" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="C11" s="22" t="s">
+      <c r="D11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A12" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="21" t="s">
+      <c r="D12" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A13" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="22" t="s">
+      <c r="D13" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="C14" s="22" t="s">
+      <c r="D14" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+      <c r="A15" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A15" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="C15" s="22" t="s">
+      <c r="D15" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A16" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
+      <c r="D16" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" s="34"/>
+        <v>133</v>
+      </c>
+      <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A20" s="17" t="s">
-        <v>69</v>
+      <c r="D19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="16" t="s">
+        <v>63</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="22" t="s">
+      <c r="A21" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="3"/>
+      <c r="D21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E22" s="34"/>
+        <v>80</v>
+      </c>
+      <c r="E22" s="33"/>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C23" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="E23" s="34"/>
+        <v>187</v>
+      </c>
+      <c r="E23" s="33"/>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>1</v>
+        <v>166</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>2</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E24" s="34"/>
+        <v>186</v>
+      </c>
+      <c r="E24" s="33"/>
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E25" s="33"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" ht="36" x14ac:dyDescent="0.15">
-      <c r="A26" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="21" t="s">
+      <c r="D26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="33"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+      <c r="A27" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:6" ht="36" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="21" t="s">
+      <c r="D27" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+    </row>
+    <row r="28" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+      <c r="A28" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D27" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-    </row>
-    <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A28" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="21" t="s">
+      <c r="D28" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A29" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A29" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="16" t="s">
+      <c r="D29" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A30" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="14"/>
-    </row>
-    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A30" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="22" t="s">
+      <c r="D30" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="13"/>
+    </row>
+    <row r="31" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="A31" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="14"/>
+      <c r="D31" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>